<commit_message>
Means of finance committed.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData4.xlsx
+++ b/src/test/resources/TestData4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_KSIDC\KSIDC_CustomerPortal-master\AI_Beacon_KSIDC_CustomerPortal\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KSIDC\AI_Beacon_KSIDC_CustomerPortal\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B30C0D0-E0F6-45AE-A80C-E199F5E8D3BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CB01C8-0CE6-4ED1-AB75-2F83B89606B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" firstSheet="21" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" firstSheet="22" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KSIDC_Registration" sheetId="11" r:id="rId1"/>
@@ -38,6 +38,7 @@
     <sheet name="KSIDC_Deposit" sheetId="34" r:id="rId23"/>
     <sheet name="KSIDC_Preliminary_Expense" sheetId="35" r:id="rId24"/>
     <sheet name="KSIDC_Technical_Know" sheetId="36" r:id="rId25"/>
+    <sheet name="KSIDC_MeansOfFinance" sheetId="37" r:id="rId26"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="416">
   <si>
     <t>Yes</t>
   </si>
@@ -1276,6 +1277,27 @@
   </si>
   <si>
     <t>45455454545</t>
+  </si>
+  <si>
+    <t>ShareCapital</t>
+  </si>
+  <si>
+    <t>InternalAccurals</t>
+  </si>
+  <si>
+    <t>UnsecuredLoan</t>
+  </si>
+  <si>
+    <t>IncentivesAndGrants</t>
+  </si>
+  <si>
+    <t>TermLoanFromOtherFI</t>
+  </si>
+  <si>
+    <t>Means of module</t>
+  </si>
+  <si>
+    <t>Test data</t>
   </si>
 </sst>
 </file>
@@ -2989,8 +3011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C3BF876-64BD-4806-8DF0-EDD78541B5B5}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3039,6 +3061,89 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221AA1B6-771A-41E2-8E7B-F141BD94A591}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>415</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
4th Commit updated xPath for 'EntrepreneursNameDropDownValue'.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData4.xlsx
+++ b/src/test/resources/TestData4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nilesh.bhoir\Documents\GitHub\AI_Beacon_KSIDC_CustomerPortal\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673858B2-5794-43EA-AC4C-8B40CE7F74DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F61637B-619E-4DC6-BBF2-13D2B61655D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11025" windowHeight="3840" firstSheet="25" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11028" windowHeight="3840" firstSheet="26" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KSIDC_Registration" sheetId="11" r:id="rId1"/>
@@ -41,6 +41,7 @@
     <sheet name="KSIDC_Sec_Misc_Fixed_Asset" sheetId="37" r:id="rId26"/>
     <sheet name="KSIDC_Sec_Corporate_Gaurantee" sheetId="38" r:id="rId27"/>
     <sheet name="KSIDC_Personal_Guarantee" sheetId="39" r:id="rId28"/>
+    <sheet name="KSIDC_Security_Summary" sheetId="40" r:id="rId29"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="413">
   <si>
     <t>Yes</t>
   </si>
@@ -1284,10 +1285,13 @@
     <t>Seurity_Misc_Fixed_Asset_Module</t>
   </si>
   <si>
-    <t>Securityt_Personal_Guarantee_Module</t>
-  </si>
-  <si>
     <t>Security_Corporate_Guarantee_Module</t>
+  </si>
+  <si>
+    <t>Security_Personal_Guarantee_Module</t>
+  </si>
+  <si>
+    <t>Security_Summary_Module</t>
   </si>
 </sst>
 </file>
@@ -1708,25 +1712,25 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="33.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="7" width="25.140625" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="7" width="25.109375" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" customWidth="1"/>
+    <col min="14" max="14" width="16.109375" customWidth="1"/>
     <col min="17" max="17" width="20" customWidth="1"/>
-    <col min="18" max="19" width="21.7109375" customWidth="1"/>
-    <col min="20" max="20" width="13.5703125" customWidth="1"/>
+    <col min="18" max="19" width="21.6640625" customWidth="1"/>
+    <col min="20" max="20" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1768,7 +1772,7 @@
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
     </row>
-    <row r="2" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1830,14 +1834,14 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1851,7 +1855,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1879,13 +1883,13 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1893,7 +1897,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1915,14 +1919,14 @@
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="24.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="19"/>
-    <col min="2" max="2" width="37.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="24.7109375" style="19"/>
+    <col min="1" max="1" width="24.6640625" style="19"/>
+    <col min="2" max="2" width="37.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="24.6640625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="18" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
@@ -1984,7 +1988,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2060,26 +2064,26 @@
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" style="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" style="20" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="20"/>
+    <col min="9" max="9" width="14.6640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.44140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.5546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>1</v>
       </c>
@@ -2123,7 +2127,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
@@ -2181,12 +2185,12 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2194,7 +2198,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2216,20 +2220,20 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2258,7 +2262,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2301,18 +2305,18 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2353,7 +2357,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2408,21 +2412,21 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2466,7 +2470,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2524,14 +2528,14 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2542,7 +2546,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2567,16 +2571,16 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2596,7 +2600,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2631,14 +2635,14 @@
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="22.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2681,7 +2685,7 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2733,13 +2737,13 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2750,7 +2754,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2775,13 +2779,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2792,7 +2796,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2817,20 +2821,20 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2877,7 +2881,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2938,13 +2942,13 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2955,7 +2959,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2980,14 +2984,14 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2998,7 +3002,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3023,16 +3027,16 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3049,7 +3053,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3081,13 +3085,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3098,7 +3102,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3119,17 +3123,17 @@
   <sheetPr codeName="Sheet27"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3140,12 +3144,12 @@
         <v>369</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>371</v>
@@ -3161,16 +3165,16 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3181,12 +3185,53 @@
         <v>369</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>410</v>
+        <v>411</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>371</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8365356-87E4-43A3-A16A-0AF790EEF51C}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>412</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>371</v>
@@ -3206,23 +3251,23 @@
       <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="26" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="26" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3275,7 +3320,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3342,29 +3387,29 @@
       <selection activeCell="O1" sqref="O1:S2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
-    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="21.42578125" customWidth="1"/>
-    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" customWidth="1"/>
+    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="21.44140625" customWidth="1"/>
+    <col min="14" max="14" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="46.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="33.88671875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3423,7 +3468,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3497,18 +3542,18 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3537,7 +3582,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3581,17 +3626,17 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="12" width="14.140625" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="14.109375" customWidth="1"/>
+    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3653,7 +3698,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3715,7 +3760,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
@@ -3736,13 +3781,13 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3750,7 +3795,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3772,30 +3817,30 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="17" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="25.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3878,7 +3923,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3975,34 +4020,34 @@
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -4130,7 +4175,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>